<commit_message>
Updated test cases and bug fixes
</commit_message>
<xml_diff>
--- a/target/run-console.xlsx
+++ b/target/run-console.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>[MYLOG]🔄 Cleared test data storage before execution.</t>
   </si>
@@ -20,268 +20,256 @@
     <t>[MYLOG] :  ?[31m************************[   MOST ACTIVE FUTURE CONTRACTS   ]*********************?[0m</t>
   </si>
   <si>
+    <t>[MYLOG] :  TATAMOTORS</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  BEL</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  TATACONSUM</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  PERSISTENT</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  TCS</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  HDFCBANK</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  TATACHEM</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  MARUTI</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  HAL</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  AMBER</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  LT</t>
+  </si>
+  <si>
     <t>[MYLOG] :  KOTAKBANK</t>
   </si>
   <si>
+    <t>[MYLOG] :  HCLTECH</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  AXISBANK</t>
+  </si>
+  <si>
     <t>[MYLOG] :  RELIANCE</t>
   </si>
   <si>
-    <t>[MYLOG] :  TATAMOTORS</t>
-  </si>
-  <si>
     <t>[MYLOG] :  INFY</t>
   </si>
   <si>
-    <t>[MYLOG] :  AXISBANK</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  LT</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  IDEA</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  TATAPOWER</t>
+    <t>[MYLOG] :  BRITANNIA</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  VEDL</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  COALINDIA</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  TRENT</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  ?[31m********************[  RISE In OI ad RISE In PRICE (BULLISH) ]*****************?[0m</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  ?[31m********************[   RISE In OI ad RISE In PRICE (BULLISH) ]*****************?[0m</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  ?[31m********************[  SLIDE In OI RISE In PRICE  (BULLISH) ]*****************?[0m</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  SHREECEM</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  ULTRACEMCO</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  MAZDOCK</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  ?[31m************************[  MOST ACTIVE STOCKS CALLS   ]*********************?[0m</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  ?[31m******************[  MOST ACTIVE STOCKS PUTS  ]********************?[0m</t>
   </si>
   <si>
     <t>[MYLOG] :  SBIN</t>
   </si>
   <si>
-    <t>[MYLOG] :  GMRAIRPORT</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  HDFCBANK</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  TCS</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  VEDL</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  BAJFINANCE</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  JSWENERGY</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  AUBANK</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ICICIBANK</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  BHARTIARTL</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  M&amp;M</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  MOTHERSON</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ?[31m********************[  RISE In OI ad RISE In PRICE (BULLISH) ]*****************?[0m</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ?[31m********************[   RISE In OI ad RISE In PRICE (BULLISH) ]*****************?[0m</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ?[31m********************[  SLIDE In OI RISE In PRICE  (BULLISH) ]*****************?[0m</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  CONCOR</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ETERNAL</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ?[31m************************[  MOST ACTIVE STOCKS CALLS   ]*********************?[0m</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  MARUTI</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  MAZDOCK</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ?[31m******************[  MOST ACTIVE STOCKS PUTS  ]********************?[0m</t>
-  </si>
-  <si>
     <t xml:space="preserve">[MYLOG] :  ****************** CHARTLINK MOMENTUM STOCKS ************************** </t>
   </si>
   <si>
-    <t>[MYLOG] :  CHOLAFIN</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  3.85%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  CYIENT</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  3.35%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  2.55%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  2.26%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  AMBER</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  2.17%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  SUPREMEIND</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.81%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.71%</t>
+    <t>[MYLOG] :  3.21%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  2.89%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  2.65%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  DALBHARAT</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  2.52%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  2.19%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  NAUKRI</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  2.12%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  BDL</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  1.94%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  1.88%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  KPITTECH</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  1.43%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  INDHOTEL</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  1.14%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  1.06%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  MPHASIS</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  1.01%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  COFORGE</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  0.93%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  SHRIRAMFIN</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  0.83%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  0.79%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  TITAGARH</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  0.75%</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  0.7%</t>
   </si>
   <si>
     <t>[MYLOG] :  BHARATFORG</t>
   </si>
   <si>
-    <t>[MYLOG] :  1.58%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  OFSS</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.47%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  UNOMINDA</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.38%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.34%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  EICHERMOT</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.33%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  JSWSTEEL</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.24%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  PRESTIGE</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.21%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.2%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  360ONE</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.16%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  MUTHOOTFIN</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.15%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  TVSMOTOR</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.14%</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  ULTRACEMCO</t>
-  </si>
-  <si>
-    <t>[MYLOG] :  1.12%</t>
-  </si>
-  <si>
-    <t>[MYLOG]✅ All Test Data Collected: [KOTAKBANK, RELIANCE, TATAMOTORS, INFY, AXISBANK, LT, IDEA, TATAPOWER, SBIN, GMRAIRPORT, HDFCBANK, TCS, VEDL, BAJFINANCE, JSWENERGY, AUBANK, ICICIBANK, BHARTIARTL, M&amp;M, MOTHERSON, LT, RELIANCE, INFY, KOTAKBANK, BHARTIARTL, CONCOR, LT, ETERNAL, GMRAIRPORT, RELIANCE, LT, KOTAKBANK, TATAPOWER, RELIANCE, TATAMOTORS, AXISBANK, SBIN, M&amp;M, MARUTI, BHARTIARTL, MAZDOCK, KOTAKBANK, RELIANCE, LT, TATAMOTORS, SBIN, MARUTI, AXISBANK, TATAPOWER, INFY]</t>
+    <t>[MYLOG] :  TATATECH</t>
+  </si>
+  <si>
+    <t>[MYLOG] :  0.67%</t>
+  </si>
+  <si>
+    <t>[MYLOG]✅ All Test Data Collected: [TATAMOTORS, BEL, TATACONSUM, PERSISTENT, TCS, HDFCBANK, TATACHEM, MARUTI, HAL, AMBER, LT, KOTAKBANK, HCLTECH, AXISBANK, RELIANCE, INFY, BRITANNIA, VEDL, COALINDIA, TRENT, HDFCBANK, RELIANCE, HAL, BEL, TATACHEM, TATAMOTORS, HCLTECH, TATACONSUM, SHREECEM, ULTRACEMCO, KOTAKBANK, MAZDOCK, HAL, BEL, PERSISTENT, LT, MAZDOCK, MARUTI, TATAMOTORS, TCS, TRENT, TATACONSUM, COALINDIA, BEL, HAL, MARUTI, SBIN, TATAMOTORS, RELIANCE, LT, TCS, PERSISTENT, KOTAKBANK]</t>
   </si>
   <si>
     <t>[MYLOG] 📊 Frequency Count:</t>
   </si>
   <si>
-    <t>[MYLOG] ICICIBANK - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] BHARTIARTL - 3</t>
-  </si>
-  <si>
-    <t>[MYLOG] MOTHERSON - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] TCS - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] MAZDOCK - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] AUBANK - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] JSWENERGY - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] TATAPOWER - 3</t>
-  </si>
-  <si>
-    <t>[MYLOG] LT - 5</t>
-  </si>
-  <si>
-    <t>[MYLOG] KOTAKBANK - 4</t>
-  </si>
-  <si>
-    <t>[MYLOG] ETERNAL - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] HDFCBANK - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] AXISBANK - 3</t>
-  </si>
-  <si>
-    <t>[MYLOG] TATAMOTORS - 3</t>
-  </si>
-  <si>
-    <t>[MYLOG] SBIN - 3</t>
-  </si>
-  <si>
-    <t>[MYLOG] MARUTI - 2</t>
-  </si>
-  <si>
-    <t>[MYLOG] M&amp;M - 2</t>
-  </si>
-  <si>
-    <t>[MYLOG] IDEA - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] CONCOR - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] BAJFINANCE - 1</t>
-  </si>
-  <si>
-    <t>[MYLOG] INFY - 3</t>
-  </si>
-  <si>
-    <t>[MYLOG] GMRAIRPORT - 2</t>
-  </si>
-  <si>
-    <t>[MYLOG] RELIANCE - 5</t>
+    <t>[MYLOG] TATACONSUM - 3</t>
+  </si>
+  <si>
+    <t>[MYLOG] PERSISTENT - 3</t>
+  </si>
+  <si>
+    <t>[MYLOG] BRITANNIA - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] TATACHEM - 2</t>
+  </si>
+  <si>
+    <t>[MYLOG] TCS - 3</t>
+  </si>
+  <si>
+    <t>[MYLOG] MAZDOCK - 2</t>
+  </si>
+  <si>
+    <t>[MYLOG] LT - 3</t>
+  </si>
+  <si>
+    <t>[MYLOG] BEL - 4</t>
+  </si>
+  <si>
+    <t>[MYLOG] KOTAKBANK - 3</t>
+  </si>
+  <si>
+    <t>[MYLOG] TRENT - 2</t>
+  </si>
+  <si>
+    <t>[MYLOG] HDFCBANK - 2</t>
+  </si>
+  <si>
+    <t>[MYLOG] HCLTECH - 2</t>
+  </si>
+  <si>
+    <t>[MYLOG] AXISBANK - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] TATAMOTORS - 4</t>
+  </si>
+  <si>
+    <t>[MYLOG] SBIN - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] SHREECEM - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] HAL - 4</t>
+  </si>
+  <si>
+    <t>[MYLOG] MARUTI - 3</t>
+  </si>
+  <si>
+    <t>[MYLOG] COALINDIA - 2</t>
+  </si>
+  <si>
+    <t>[MYLOG] AMBER - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] INFY - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] ULTRACEMCO - 1</t>
+  </si>
+  <si>
+    <t>[MYLOG] RELIANCE - 3</t>
   </si>
   <si>
     <t>[MYLOG] VEDL - 1</t>
@@ -329,7 +317,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A131"/>
+  <dimension ref="A1:A146"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -355,127 +343,127 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
@@ -485,62 +473,62 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -550,447 +538,522 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="0">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="0">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="0">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="0">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="0">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="0">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="0">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s" s="0">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s" s="0">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s" s="0">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="0">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s" s="0">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="0">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s" s="0">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="0">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="0">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s" s="0">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s" s="0">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s" s="0">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s" s="0">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s" s="0">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="0">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="0">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s" s="0">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="0">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s" s="0">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s" s="0">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s" s="0">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s" s="0">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s" s="0">
-        <v>67</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s" s="0">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s" s="0">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s" s="0">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s" s="0">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s" s="0">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s" s="0">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s" s="0">
-        <v>75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s" s="0">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s" s="0">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s" s="0">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s" s="0">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s" s="0">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s" s="0">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s" s="0">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s" s="0">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s" s="0">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s" s="0">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s" s="0">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s" s="0">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s" s="0">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s" s="0">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s" s="0">
-        <v>90</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="0">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="0">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="0">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="0">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>